<commit_message>
changed the amazon account details in excel sheet
</commit_message>
<xml_diff>
--- a/SpecFrame/FeatureFiles/specflowdata.xlsx
+++ b/SpecFrame/FeatureFiles/specflowdata.xlsx
@@ -39,12 +39,6 @@
     <t>exactitem</t>
   </si>
   <si>
-    <t xml:space="preserve">nandyupali@gmail.com </t>
-  </si>
-  <si>
-    <t>ganesha123</t>
-  </si>
-  <si>
     <t xml:space="preserve">iphone </t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>Amazon.in: moto g4 plus - Smartphones / Smartphones &amp; Basic Mobiles: Electronics</t>
+  </si>
+  <si>
+    <t>testdemo372@gmail.com</t>
+  </si>
+  <si>
+    <t>india123</t>
   </si>
 </sst>
 </file>
@@ -398,12 +398,12 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
@@ -433,42 +433,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the amazon account username password in excel sheet
</commit_message>
<xml_diff>
--- a/SpecFrame/FeatureFiles/specflowdata.xlsx
+++ b/SpecFrame/FeatureFiles/specflowdata.xlsx
@@ -63,10 +63,10 @@
     <t>Amazon.in: moto g4 plus - Smartphones / Smartphones &amp; Basic Mobiles: Electronics</t>
   </si>
   <si>
-    <t>testdemo372@gmail.com</t>
-  </si>
-  <si>
-    <t>india123</t>
+    <t>nandyupali@gmail.com</t>
+  </si>
+  <si>
+    <t>ganesha123</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>